<commit_message>
Updated to include 12 count 4333 mirrors
</commit_message>
<xml_diff>
--- a/investigateNTor4M/output/summary.xlsx
+++ b/investigateNTor4M/output/summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="14355" windowHeight="11565"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="14355" windowHeight="11565" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="8-15" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="22">
   <si>
     <t>NT hand</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>d2000</t>
+  </si>
+  <si>
+    <t>d5000</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -1223,23 +1226,23 @@
         <v>19</v>
       </c>
       <c r="K6">
-        <f>RANK(F6,$F$6:$F$21)</f>
+        <f t="shared" ref="K6:K20" si="0">RANK(F6,$F$6:$F$21)</f>
         <v>2</v>
       </c>
       <c r="L6">
-        <f>RANK(H6,$H$6:$H$21)</f>
+        <f t="shared" ref="L6:L20" si="1">RANK(H6,$H$6:$H$21)</f>
         <v>1</v>
       </c>
       <c r="M6">
-        <f>RANK(I6,$I$6:$I$21)</f>
+        <f t="shared" ref="M6:M20" si="2">RANK(I6,$I$6:$I$21)</f>
         <v>1</v>
       </c>
       <c r="O6">
-        <f>SUM(K6:M6)</f>
+        <f t="shared" ref="O6:O20" si="3">SUM(K6:M6)</f>
         <v>4</v>
       </c>
       <c r="Q6">
-        <f>RANK(O6,$O$6:$O$21,1)</f>
+        <f t="shared" ref="Q6:Q20" si="4">RANK(O6,$O$6:$O$21,1)</f>
         <v>1</v>
       </c>
     </row>
@@ -1269,23 +1272,23 @@
         <v>19</v>
       </c>
       <c r="K7">
-        <f>RANK(F7,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L7">
-        <f>RANK(H7,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="M7">
-        <f>RANK(I7,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O7">
-        <f>SUM(K7:M7)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="Q7">
-        <f>RANK(O7,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -1315,23 +1318,23 @@
         <v>19</v>
       </c>
       <c r="K8">
-        <f>RANK(F8,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L8">
-        <f>RANK(H8,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="M8">
-        <f>RANK(I8,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O8">
-        <f>SUM(K8:M8)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="Q8">
-        <f>RANK(O8,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -1361,23 +1364,23 @@
         <v>19</v>
       </c>
       <c r="K9">
-        <f>RANK(F9,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L9">
-        <f>RANK(H9,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="M9">
-        <f>RANK(I9,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="O9">
-        <f>SUM(K9:M9)</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="Q9">
-        <f>RANK(O9,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
@@ -1407,23 +1410,23 @@
         <v>19</v>
       </c>
       <c r="K10">
-        <f>RANK(F10,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="L10">
-        <f>RANK(H10,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="M10">
-        <f>RANK(I10,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="O10">
-        <f>SUM(K10:M10)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="Q10">
-        <f>RANK(O10,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -1453,23 +1456,23 @@
         <v>19</v>
       </c>
       <c r="K11">
-        <f>RANK(F11,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L11">
-        <f>RANK(H11,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="M11">
-        <f>RANK(I11,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="O11">
-        <f>SUM(K11:M11)</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="Q11">
-        <f>RANK(O11,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
     </row>
@@ -1499,23 +1502,23 @@
         <v>19</v>
       </c>
       <c r="K12">
-        <f>RANK(F12,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L12">
-        <f>RANK(H12,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="M12">
-        <f>RANK(I12,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="O12">
-        <f>SUM(K12:M12)</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="Q12">
-        <f>RANK(O12,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
     </row>
@@ -1545,23 +1548,23 @@
         <v>19</v>
       </c>
       <c r="K13">
-        <f>RANK(F13,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L13">
-        <f>RANK(H13,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="M13">
-        <f>RANK(I13,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="O13">
-        <f>SUM(K13:M13)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="Q13">
-        <f>RANK(O13,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
     </row>
@@ -1591,23 +1594,23 @@
         <v>19</v>
       </c>
       <c r="K14">
-        <f>RANK(F14,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L14">
-        <f>RANK(H14,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="M14">
-        <f>RANK(I14,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="O14">
-        <f>SUM(K14:M14)</f>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="Q14">
-        <f>RANK(O14,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
@@ -1637,23 +1640,23 @@
         <v>19</v>
       </c>
       <c r="K15">
-        <f>RANK(F15,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L15">
-        <f>RANK(H15,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M15">
-        <f>RANK(I15,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="O15">
-        <f>SUM(K15:M15)</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="Q15">
-        <f>RANK(O15,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
     </row>
@@ -1683,23 +1686,23 @@
         <v>19</v>
       </c>
       <c r="K16">
-        <f>RANK(F16,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="L16">
-        <f>RANK(H16,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="M16">
-        <f>RANK(I16,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="O16">
-        <f>SUM(K16:M16)</f>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="Q16">
-        <f>RANK(O16,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
@@ -1729,23 +1732,23 @@
         <v>19</v>
       </c>
       <c r="K17">
-        <f>RANK(F17,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="L17">
-        <f>RANK(H17,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="M17">
-        <f>RANK(I17,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="O17">
-        <f>SUM(K17:M17)</f>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="Q17">
-        <f>RANK(O17,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -1775,23 +1778,23 @@
         <v>19</v>
       </c>
       <c r="K18">
-        <f>RANK(F18,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="L18">
-        <f>RANK(H18,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="M18">
-        <f>RANK(I18,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="O18">
-        <f>SUM(K18:M18)</f>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="Q18">
-        <f>RANK(O18,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
     </row>
@@ -1821,23 +1824,23 @@
         <v>19</v>
       </c>
       <c r="K19">
-        <f>RANK(F19,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="L19">
-        <f>RANK(H19,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="M19">
-        <f>RANK(I19,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="O19">
-        <f>SUM(K19:M19)</f>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="Q19">
-        <f>RANK(O19,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
     </row>
@@ -1867,23 +1870,23 @@
         <v>19</v>
       </c>
       <c r="K20">
-        <f>RANK(F20,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="L20">
-        <f>RANK(H20,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M20">
-        <f>RANK(I20,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="O20">
-        <f>SUM(K20:M20)</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="Q20">
-        <f>RANK(O20,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
     </row>
@@ -1899,8 +1902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:Q20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1983,23 +1986,23 @@
         <v>19</v>
       </c>
       <c r="K6">
-        <f>RANK(F6,$F$6:$F$21)</f>
+        <f t="shared" ref="K6:K20" si="0">RANK(F6,$F$6:$F$21)</f>
         <v>1</v>
       </c>
       <c r="L6">
-        <f>RANK(H6,$H$6:$H$21)</f>
+        <f t="shared" ref="L6:L20" si="1">RANK(H6,$H$6:$H$21)</f>
         <v>1</v>
       </c>
       <c r="M6">
-        <f>RANK(I6,$I$6:$I$21)</f>
+        <f t="shared" ref="M6:M20" si="2">RANK(I6,$I$6:$I$21)</f>
         <v>1</v>
       </c>
       <c r="O6">
-        <f>SUM(K6:M6)</f>
+        <f t="shared" ref="O6:O20" si="3">SUM(K6:M6)</f>
         <v>3</v>
       </c>
       <c r="Q6">
-        <f>RANK(O6,$O$6:$O$21,1)</f>
+        <f t="shared" ref="Q6:Q20" si="4">RANK(O6,$O$6:$O$21,1)</f>
         <v>1</v>
       </c>
     </row>
@@ -2029,23 +2032,23 @@
         <v>19</v>
       </c>
       <c r="K7">
-        <f>RANK(F7,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L7">
-        <f>RANK(H7,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="M7">
-        <f>RANK(I7,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O7">
-        <f>SUM(K7:M7)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="Q7">
-        <f>RANK(O7,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -2075,23 +2078,23 @@
         <v>19</v>
       </c>
       <c r="K8">
-        <f>RANK(F8,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L8">
-        <f>RANK(H8,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="M8">
-        <f>RANK(I8,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O8">
-        <f>SUM(K8:M8)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="Q8">
-        <f>RANK(O8,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -2121,23 +2124,23 @@
         <v>19</v>
       </c>
       <c r="K9">
-        <f>RANK(F9,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L9">
-        <f>RANK(H9,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="M9">
-        <f>RANK(I9,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="O9">
-        <f>SUM(K9:M9)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="Q9">
-        <f>RANK(O9,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
@@ -2167,23 +2170,23 @@
         <v>19</v>
       </c>
       <c r="K10">
-        <f>RANK(F10,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L10">
-        <f>RANK(H10,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="M10">
-        <f>RANK(I10,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="O10">
-        <f>SUM(K10:M10)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="Q10">
-        <f>RANK(O10,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -2213,23 +2216,23 @@
         <v>19</v>
       </c>
       <c r="K11">
-        <f>RANK(F11,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L11">
-        <f>RANK(H11,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="M11">
-        <f>RANK(I11,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="O11">
-        <f>SUM(K11:M11)</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="Q11">
-        <f>RANK(O11,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
     </row>
@@ -2259,23 +2262,23 @@
         <v>19</v>
       </c>
       <c r="K12">
-        <f>RANK(F12,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L12">
-        <f>RANK(H12,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="M12">
-        <f>RANK(I12,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="O12">
-        <f>SUM(K12:M12)</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="Q12">
-        <f>RANK(O12,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
     </row>
@@ -2305,23 +2308,23 @@
         <v>19</v>
       </c>
       <c r="K13">
-        <f>RANK(F13,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="L13">
-        <f>RANK(H13,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="M13">
-        <f>RANK(I13,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="O13">
-        <f>SUM(K13:M13)</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="Q13">
-        <f>RANK(O13,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
     </row>
@@ -2351,23 +2354,23 @@
         <v>19</v>
       </c>
       <c r="K14">
-        <f>RANK(F14,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L14">
-        <f>RANK(H14,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="M14">
-        <f>RANK(I14,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="O14">
-        <f>SUM(K14:M14)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="Q14">
-        <f>RANK(O14,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
@@ -2397,23 +2400,23 @@
         <v>19</v>
       </c>
       <c r="K15">
-        <f>RANK(F15,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L15">
-        <f>RANK(H15,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="M15">
-        <f>RANK(I15,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="O15">
-        <f>SUM(K15:M15)</f>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="Q15">
-        <f>RANK(O15,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
     </row>
@@ -2443,23 +2446,23 @@
         <v>19</v>
       </c>
       <c r="K16">
-        <f>RANK(F16,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="L16">
-        <f>RANK(H16,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M16">
-        <f>RANK(I16,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="O16">
-        <f>SUM(K16:M16)</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="Q16">
-        <f>RANK(O16,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
@@ -2489,23 +2492,23 @@
         <v>19</v>
       </c>
       <c r="K17">
-        <f>RANK(F17,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="L17">
-        <f>RANK(H17,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="M17">
-        <f>RANK(I17,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="O17">
-        <f>SUM(K17:M17)</f>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="Q17">
-        <f>RANK(O17,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -2535,23 +2538,23 @@
         <v>19</v>
       </c>
       <c r="K18">
-        <f>RANK(F18,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="L18">
-        <f>RANK(H18,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="M18">
-        <f>RANK(I18,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="O18">
-        <f>SUM(K18:M18)</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="Q18">
-        <f>RANK(O18,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
     </row>
@@ -2581,23 +2584,23 @@
         <v>19</v>
       </c>
       <c r="K19">
-        <f>RANK(F19,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="L19">
-        <f>RANK(H19,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="M19">
-        <f>RANK(I19,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="O19">
-        <f>SUM(K19:M19)</f>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="Q19">
-        <f>RANK(O19,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
     </row>
@@ -2612,35 +2615,38 @@
         <v>11</v>
       </c>
       <c r="F20">
-        <v>20.7</v>
+        <v>20.6</v>
       </c>
       <c r="G20">
-        <v>79.3</v>
+        <v>79.400000000000006</v>
       </c>
       <c r="H20">
-        <v>-3.0516999999999999</v>
+        <v>-3.125</v>
       </c>
       <c r="I20">
-        <v>-3.9089999999999998</v>
+        <v>-3.8041999999999998</v>
+      </c>
+      <c r="J20" t="s">
+        <v>21</v>
       </c>
       <c r="K20">
-        <f>RANK(F20,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="L20">
-        <f>RANK(H20,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M20">
-        <f>RANK(I20,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="O20">
-        <f>SUM(K20:M20)</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="Q20">
-        <f>RANK(O20,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
     </row>
@@ -2740,23 +2746,23 @@
         <v>20</v>
       </c>
       <c r="K6">
-        <f>RANK(F6,$F$6:$F$21)</f>
+        <f t="shared" ref="K6:K20" si="0">RANK(F6,$F$6:$F$21)</f>
         <v>1</v>
       </c>
       <c r="L6">
-        <f>RANK(H6,$H$6:$H$21)</f>
+        <f t="shared" ref="L6:L20" si="1">RANK(H6,$H$6:$H$21)</f>
         <v>1</v>
       </c>
       <c r="M6">
-        <f>RANK(I6,$I$6:$I$21)</f>
+        <f t="shared" ref="M6:M20" si="2">RANK(I6,$I$6:$I$21)</f>
         <v>1</v>
       </c>
       <c r="O6">
-        <f>SUM(K6:M6)</f>
+        <f t="shared" ref="O6:O20" si="3">SUM(K6:M6)</f>
         <v>3</v>
       </c>
       <c r="Q6">
-        <f>RANK(O6,$O$6:$O$21,1)</f>
+        <f t="shared" ref="Q6:Q20" si="4">RANK(O6,$O$6:$O$21,1)</f>
         <v>1</v>
       </c>
     </row>
@@ -2786,23 +2792,23 @@
         <v>19</v>
       </c>
       <c r="K7">
-        <f>RANK(F7,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L7">
-        <f>RANK(H7,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="M7">
-        <f>RANK(I7,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O7">
-        <f>SUM(K7:M7)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="Q7">
-        <f>RANK(O7,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -2832,23 +2838,23 @@
         <v>19</v>
       </c>
       <c r="K8">
-        <f>RANK(F8,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L8">
-        <f>RANK(H8,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="M8">
-        <f>RANK(I8,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O8">
-        <f>SUM(K8:M8)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="Q8">
-        <f>RANK(O8,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -2878,23 +2884,23 @@
         <v>19</v>
       </c>
       <c r="K9">
-        <f>RANK(F9,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L9">
-        <f>RANK(H9,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="M9">
-        <f>RANK(I9,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="O9">
-        <f>SUM(K9:M9)</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="Q9">
-        <f>RANK(O9,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
@@ -2924,23 +2930,23 @@
         <v>19</v>
       </c>
       <c r="K10">
-        <f>RANK(F10,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L10">
-        <f>RANK(H10,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="M10">
-        <f>RANK(I10,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="O10">
-        <f>SUM(K10:M10)</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="Q10">
-        <f>RANK(O10,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -2970,23 +2976,23 @@
         <v>19</v>
       </c>
       <c r="K11">
-        <f>RANK(F11,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L11">
-        <f>RANK(H11,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="M11">
-        <f>RANK(I11,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="O11">
-        <f>SUM(K11:M11)</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="Q11">
-        <f>RANK(O11,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
     </row>
@@ -3016,23 +3022,23 @@
         <v>19</v>
       </c>
       <c r="K12">
-        <f>RANK(F12,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L12">
-        <f>RANK(H12,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="M12">
-        <f>RANK(I12,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="O12">
-        <f>SUM(K12:M12)</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="Q12">
-        <f>RANK(O12,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
     </row>
@@ -3062,23 +3068,23 @@
         <v>19</v>
       </c>
       <c r="K13">
-        <f>RANK(F13,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="L13">
-        <f>RANK(H13,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M13">
-        <f>RANK(I13,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="O13">
-        <f>SUM(K13:M13)</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="Q13">
-        <f>RANK(O13,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
     </row>
@@ -3108,23 +3114,23 @@
         <v>19</v>
       </c>
       <c r="K14">
-        <f>RANK(F14,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L14">
-        <f>RANK(H14,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="M14">
-        <f>RANK(I14,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="O14">
-        <f>SUM(K14:M14)</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="Q14">
-        <f>RANK(O14,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
@@ -3154,23 +3160,23 @@
         <v>19</v>
       </c>
       <c r="K15">
-        <f>RANK(F15,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L15">
-        <f>RANK(H15,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="M15">
-        <f>RANK(I15,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="O15">
-        <f>SUM(K15:M15)</f>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="Q15">
-        <f>RANK(O15,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
     </row>
@@ -3200,23 +3206,23 @@
         <v>20</v>
       </c>
       <c r="K16">
-        <f>RANK(F16,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="L16">
-        <f>RANK(H16,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="M16">
-        <f>RANK(I16,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="O16">
-        <f>SUM(K16:M16)</f>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="Q16">
-        <f>RANK(O16,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
@@ -3246,23 +3252,23 @@
         <v>20</v>
       </c>
       <c r="K17">
-        <f>RANK(F17,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="L17">
-        <f>RANK(H17,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="M17">
-        <f>RANK(I17,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="O17">
-        <f>SUM(K17:M17)</f>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="Q17">
-        <f>RANK(O17,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -3292,23 +3298,23 @@
         <v>19</v>
       </c>
       <c r="K18">
-        <f>RANK(F18,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="L18">
-        <f>RANK(H18,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="M18">
-        <f>RANK(I18,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="O18">
-        <f>SUM(K18:M18)</f>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="Q18">
-        <f>RANK(O18,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
     </row>
@@ -3338,23 +3344,23 @@
         <v>19</v>
       </c>
       <c r="K19">
-        <f>RANK(F19,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="L19">
-        <f>RANK(H19,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="M19">
-        <f>RANK(I19,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="O19">
-        <f>SUM(K19:M19)</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="Q19">
-        <f>RANK(O19,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
     </row>
@@ -3384,23 +3390,23 @@
         <v>20</v>
       </c>
       <c r="K20">
-        <f>RANK(F20,$F$6:$F$21)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="L20">
-        <f>RANK(H20,$H$6:$H$21)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M20">
-        <f>RANK(I20,$I$6:$I$21)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="O20">
-        <f>SUM(K20:M20)</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="Q20">
-        <f>RANK(O20,$O$6:$O$21,1)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
     </row>

</xml_diff>